<commit_message>
Daily attendance processing - 2026-02-07 12:49:10 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>77.6%</t>
+          <t>78.6%</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>72.5%</t>
+          <t>72.2%</t>
         </is>
       </c>
     </row>
@@ -1603,22 +1603,22 @@
         <v>40</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P19" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q19" s="4" t="n">
         <v>4</v>
       </c>
       <c r="R19" s="4" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>82.5%</t>
         </is>
       </c>
       <c r="S19" s="4" t="inlineStr">
         <is>
-          <t>71.3%</t>
+          <t>71.5%</t>
         </is>
       </c>
     </row>
@@ -1681,22 +1681,22 @@
         <v>42</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P20" s="4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q20" s="4" t="n">
         <v>4</v>
       </c>
       <c r="R20" s="4" t="inlineStr">
         <is>
-          <t>71.4%</t>
+          <t>73.8%</t>
         </is>
       </c>
       <c r="S20" s="4" t="inlineStr">
         <is>
-          <t>77.8%</t>
+          <t>75.4%</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
         <v>40</v>
       </c>
       <c r="O22" s="4" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P22" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="4" t="n">
         <v>4</v>
       </c>
       <c r="R22" s="4" t="inlineStr">
         <is>
-          <t>82.5%</t>
+          <t>85.0%</t>
         </is>
       </c>
       <c r="S22" s="4" t="inlineStr">
@@ -8544,45 +8544,45 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B177" s="5" t="inlineStr">
+      <c r="A177" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B177" s="2" t="inlineStr">
         <is>
           <t>B2-C1</t>
         </is>
       </c>
-      <c r="C177" s="5" t="inlineStr">
+      <c r="C177" s="2" t="inlineStr">
         <is>
           <t>GASTROENTEROLOGY</t>
         </is>
       </c>
-      <c r="D177" s="5" t="inlineStr">
+      <c r="D177" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E177" s="5" t="inlineStr">
+      <c r="E177" s="2" t="inlineStr">
         <is>
           <t>07/02/2026</t>
         </is>
       </c>
-      <c r="F177" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G177" s="5" t="inlineStr"/>
-      <c r="H177" s="5" t="inlineStr">
-        <is>
-          <t>0/52</t>
-        </is>
-      </c>
-      <c r="I177" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F177" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G177" s="2" t="inlineStr"/>
+      <c r="H177" s="2" t="inlineStr">
+        <is>
+          <t>40/52</t>
+        </is>
+      </c>
+      <c r="I177" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -10264,45 +10264,45 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B217" s="5" t="inlineStr">
+      <c r="A217" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B217" s="2" t="inlineStr">
         <is>
           <t>B2-C2</t>
         </is>
       </c>
-      <c r="C217" s="5" t="inlineStr">
+      <c r="C217" s="2" t="inlineStr">
         <is>
           <t>GASTROENTEROLOGY</t>
         </is>
       </c>
-      <c r="D217" s="5" t="inlineStr">
+      <c r="D217" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E217" s="5" t="inlineStr">
+      <c r="E217" s="2" t="inlineStr">
         <is>
           <t>07/02/2026</t>
         </is>
       </c>
-      <c r="F217" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G217" s="5" t="inlineStr"/>
-      <c r="H217" s="5" t="inlineStr">
-        <is>
-          <t>0/51</t>
-        </is>
-      </c>
-      <c r="I217" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F217" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G217" s="2" t="inlineStr"/>
+      <c r="H217" s="2" t="inlineStr">
+        <is>
+          <t>2/51</t>
+        </is>
+      </c>
+      <c r="I217" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -14650,45 +14650,45 @@
       </c>
     </row>
     <row r="319">
-      <c r="A319" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B319" s="5" t="inlineStr">
+      <c r="A319" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B319" s="2" t="inlineStr">
         <is>
           <t>B2-D2</t>
         </is>
       </c>
-      <c r="C319" s="5" t="inlineStr">
+      <c r="C319" s="2" t="inlineStr">
         <is>
           <t>RHEUMATOLOGY</t>
         </is>
       </c>
-      <c r="D319" s="5" t="inlineStr">
+      <c r="D319" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E319" s="5" t="inlineStr">
+      <c r="E319" s="2" t="inlineStr">
         <is>
           <t>07/02/2026</t>
         </is>
       </c>
-      <c r="F319" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G319" s="5" t="inlineStr"/>
-      <c r="H319" s="5" t="inlineStr">
-        <is>
-          <t>0/61</t>
-        </is>
-      </c>
-      <c r="I319" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F319" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G319" s="2" t="inlineStr"/>
+      <c r="H319" s="2" t="inlineStr">
+        <is>
+          <t>34/61</t>
+        </is>
+      </c>
+      <c r="I319" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 09:09:12 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>78.6%</t>
+          <t>78.9%</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>72.2%</t>
+          <t>72.0%</t>
         </is>
       </c>
     </row>
@@ -1603,22 +1603,22 @@
         <v>40</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P19" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q19" s="4" t="n">
         <v>3</v>
       </c>
       <c r="R19" s="4" t="inlineStr">
         <is>
-          <t>82.5%</t>
+          <t>85.0%</t>
         </is>
       </c>
       <c r="S19" s="4" t="inlineStr">
         <is>
-          <t>71.5%</t>
+          <t>70.0%</t>
         </is>
       </c>
     </row>
@@ -8587,45 +8587,45 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B178" s="5" t="inlineStr">
+      <c r="A178" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B178" s="2" t="inlineStr">
         <is>
           <t>B2-C1</t>
         </is>
       </c>
-      <c r="C178" s="5" t="inlineStr">
+      <c r="C178" s="2" t="inlineStr">
         <is>
           <t>GASTROENTEROLOGY</t>
         </is>
       </c>
-      <c r="D178" s="5" t="inlineStr">
+      <c r="D178" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E178" s="5" t="inlineStr">
+      <c r="E178" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F178" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G178" s="5" t="inlineStr"/>
-      <c r="H178" s="5" t="inlineStr">
-        <is>
-          <t>0/52</t>
-        </is>
-      </c>
-      <c r="I178" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F178" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G178" s="2" t="inlineStr"/>
+      <c r="H178" s="2" t="inlineStr">
+        <is>
+          <t>11/52</t>
+        </is>
+      </c>
+      <c r="I178" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 11:04:29 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -487,7 +487,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="23" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>78.9%</t>
+          <t>79.8%</t>
         </is>
       </c>
     </row>
@@ -1291,17 +1291,17 @@
         <v>40</v>
       </c>
       <c r="O15" s="4" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P15" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="4" t="n">
         <v>3</v>
       </c>
       <c r="R15" s="4" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>82.5%</t>
         </is>
       </c>
       <c r="S15" s="4" t="inlineStr">
@@ -1369,22 +1369,22 @@
         <v>40</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P16" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q16" s="4" t="n">
         <v>3</v>
       </c>
       <c r="R16" s="4" t="inlineStr">
         <is>
-          <t>77.5%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="S16" s="4" t="inlineStr">
         <is>
-          <t>83.9%</t>
+          <t>83.4%</t>
         </is>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="S19" s="4" t="inlineStr">
         <is>
-          <t>70.0%</t>
+          <t>71.9%</t>
         </is>
       </c>
     </row>
@@ -1681,22 +1681,22 @@
         <v>42</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P20" s="4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q20" s="4" t="n">
         <v>3</v>
       </c>
       <c r="R20" s="4" t="inlineStr">
         <is>
-          <t>73.8%</t>
+          <t>76.2%</t>
         </is>
       </c>
       <c r="S20" s="4" t="inlineStr">
         <is>
-          <t>75.4%</t>
+          <t>73.1%</t>
         </is>
       </c>
     </row>
@@ -2309,45 +2309,49 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B32" s="5" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
         <is>
           <t>B2-A1</t>
         </is>
       </c>
-      <c r="C32" s="5" t="inlineStr">
+      <c r="C32" s="2" t="inlineStr">
         <is>
           <t>NEUROLOGY</t>
         </is>
       </c>
-      <c r="D32" s="5" t="inlineStr">
+      <c r="D32" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E32" s="5" t="inlineStr">
+      <c r="E32" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F32" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G32" s="5" t="inlineStr"/>
-      <c r="H32" s="5" t="inlineStr">
-        <is>
-          <t>0/25</t>
-        </is>
-      </c>
-      <c r="I32" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>160715@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>20/25</t>
+        </is>
+      </c>
+      <c r="I32" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -4029,45 +4033,49 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B72" s="5" t="inlineStr">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
         <is>
           <t>B2-A2</t>
         </is>
       </c>
-      <c r="C72" s="5" t="inlineStr">
+      <c r="C72" s="2" t="inlineStr">
         <is>
           <t>NEUROLOGY</t>
         </is>
       </c>
-      <c r="D72" s="5" t="inlineStr">
+      <c r="D72" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E72" s="5" t="inlineStr">
+      <c r="E72" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F72" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G72" s="5" t="inlineStr"/>
-      <c r="H72" s="5" t="inlineStr">
-        <is>
-          <t>0/23</t>
-        </is>
-      </c>
-      <c r="I72" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F72" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G72" s="2" t="inlineStr">
+        <is>
+          <t>160715@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H72" s="2" t="inlineStr">
+        <is>
+          <t>16/23</t>
+        </is>
+      </c>
+      <c r="I72" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -8620,7 +8628,7 @@
       <c r="G178" s="2" t="inlineStr"/>
       <c r="H178" s="2" t="inlineStr">
         <is>
-          <t>11/52</t>
+          <t>45/52</t>
         </is>
       </c>
       <c r="I178" s="2" t="inlineStr">
@@ -10307,45 +10315,45 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B218" s="5" t="inlineStr">
+      <c r="A218" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B218" s="2" t="inlineStr">
         <is>
           <t>B2-C2</t>
         </is>
       </c>
-      <c r="C218" s="5" t="inlineStr">
+      <c r="C218" s="2" t="inlineStr">
         <is>
           <t>GASTROENTEROLOGY</t>
         </is>
       </c>
-      <c r="D218" s="5" t="inlineStr">
+      <c r="D218" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E218" s="5" t="inlineStr">
+      <c r="E218" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F218" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G218" s="5" t="inlineStr"/>
-      <c r="H218" s="5" t="inlineStr">
-        <is>
-          <t>0/51</t>
-        </is>
-      </c>
-      <c r="I218" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F218" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G218" s="2" t="inlineStr"/>
+      <c r="H218" s="2" t="inlineStr">
+        <is>
+          <t>1/51</t>
+        </is>
+      </c>
+      <c r="I218" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 13:52:30 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -1774,7 +1774,7 @@
       </c>
       <c r="S21" s="4" t="inlineStr">
         <is>
-          <t>70.4%</t>
+          <t>70.6%</t>
         </is>
       </c>
     </row>
@@ -12381,7 +12381,7 @@
       </c>
       <c r="H265" s="2" t="inlineStr">
         <is>
-          <t>14/28</t>
+          <t>15/28</t>
         </is>
       </c>
       <c r="I265" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 20:33:10 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -2195,7 +2195,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G29" s="2" t="inlineStr"/>
+      <c r="G29" s="2" t="inlineStr">
+        <is>
+          <t>160715@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
           <t>25/25</t>
@@ -3934,7 +3938,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G69" s="2" t="inlineStr"/>
+      <c r="G69" s="2" t="inlineStr">
+        <is>
+          <t>160715@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H69" s="2" t="inlineStr">
         <is>
           <t>18/23</t>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-09 09:42:06 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>80.4%</t>
+          <t>80.7%</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>72.1%</t>
+          <t>71.9%</t>
         </is>
       </c>
     </row>
@@ -1837,22 +1837,22 @@
         <v>40</v>
       </c>
       <c r="O22" s="4" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P22" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="4" t="n">
         <v>2</v>
       </c>
       <c r="R22" s="4" t="inlineStr">
         <is>
-          <t>87.5%</t>
+          <t>90.0%</t>
         </is>
       </c>
       <c r="S22" s="4" t="inlineStr">
         <is>
-          <t>56.4%</t>
+          <t>55.4%</t>
         </is>
       </c>
     </row>
@@ -14764,45 +14764,45 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B321" s="5" t="inlineStr">
+      <c r="A321" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B321" s="2" t="inlineStr">
         <is>
           <t>B2-D2</t>
         </is>
       </c>
-      <c r="C321" s="5" t="inlineStr">
+      <c r="C321" s="2" t="inlineStr">
         <is>
           <t>RHEUMATOLOGY</t>
         </is>
       </c>
-      <c r="D321" s="5" t="inlineStr">
+      <c r="D321" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E321" s="5" t="inlineStr">
+      <c r="E321" s="2" t="inlineStr">
         <is>
           <t>09/02/2026</t>
         </is>
       </c>
-      <c r="F321" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G321" s="5" t="inlineStr"/>
-      <c r="H321" s="5" t="inlineStr">
-        <is>
-          <t>0/61</t>
-        </is>
-      </c>
-      <c r="I321" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F321" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G321" s="2" t="inlineStr"/>
+      <c r="H321" s="2" t="inlineStr">
+        <is>
+          <t>11/61</t>
+        </is>
+      </c>
+      <c r="I321" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-10 06:21:21 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>82.9%</t>
+          <t>83.5%</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>71.8%</t>
+          <t>71.9%</t>
         </is>
       </c>
     </row>
@@ -1447,22 +1447,22 @@
         <v>40</v>
       </c>
       <c r="O17" s="4" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P17" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q17" s="4" t="n">
         <v>2</v>
       </c>
       <c r="R17" s="4" t="inlineStr">
         <is>
-          <t>87.5%</t>
+          <t>90.0%</t>
         </is>
       </c>
       <c r="S17" s="4" t="inlineStr">
         <is>
-          <t>71.9%</t>
+          <t>71.8%</t>
         </is>
       </c>
     </row>
@@ -1525,22 +1525,22 @@
         <v>40</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P18" s="4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q18" s="4" t="n">
         <v>2</v>
       </c>
       <c r="R18" s="4" t="inlineStr">
         <is>
-          <t>77.5%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="S18" s="4" t="inlineStr">
         <is>
-          <t>69.1%</t>
+          <t>70.0%</t>
         </is>
       </c>
     </row>
@@ -4757,45 +4757,45 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B88" s="5" t="inlineStr">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
         <is>
           <t>B2-B1</t>
         </is>
       </c>
-      <c r="C88" s="5" t="inlineStr">
+      <c r="C88" s="2" t="inlineStr">
         <is>
           <t>ENDOCRINOLOGY</t>
         </is>
       </c>
-      <c r="D88" s="5" t="inlineStr">
+      <c r="D88" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E88" s="5" t="inlineStr">
+      <c r="E88" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F88" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G88" s="5" t="inlineStr"/>
-      <c r="H88" s="5" t="inlineStr">
-        <is>
-          <t>0/40</t>
-        </is>
-      </c>
-      <c r="I88" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F88" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G88" s="2" t="inlineStr"/>
+      <c r="H88" s="2" t="inlineStr">
+        <is>
+          <t>27/40</t>
+        </is>
+      </c>
+      <c r="I88" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -6497,45 +6497,45 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B128" s="5" t="inlineStr">
+      <c r="A128" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B128" s="2" t="inlineStr">
         <is>
           <t>B2-B2</t>
         </is>
       </c>
-      <c r="C128" s="5" t="inlineStr">
+      <c r="C128" s="2" t="inlineStr">
         <is>
           <t>ENDOCRINOLOGY</t>
         </is>
       </c>
-      <c r="D128" s="5" t="inlineStr">
+      <c r="D128" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E128" s="5" t="inlineStr">
+      <c r="E128" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F128" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G128" s="5" t="inlineStr"/>
-      <c r="H128" s="5" t="inlineStr">
-        <is>
-          <t>0/35</t>
-        </is>
-      </c>
-      <c r="I128" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F128" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G128" s="2" t="inlineStr"/>
+      <c r="H128" s="2" t="inlineStr">
+        <is>
+          <t>34/35</t>
+        </is>
+      </c>
+      <c r="I128" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 11:52:51 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8">
@@ -950,7 +950,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>85.1%</t>
+          <t>85.4%</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>71.5%</t>
+          <t>71.4%</t>
         </is>
       </c>
     </row>
@@ -1834,22 +1834,22 @@
         <v>40</v>
       </c>
       <c r="O22" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P22" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R22" s="4" t="inlineStr">
         <is>
-          <t>92.5%</t>
+          <t>95.0%</t>
         </is>
       </c>
       <c r="S22" s="4" t="inlineStr">
         <is>
-          <t>55.1%</t>
+          <t>55.2%</t>
         </is>
       </c>
     </row>
@@ -14923,45 +14923,45 @@
       </c>
     </row>
     <row r="323">
-      <c r="A323" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B323" s="5" t="inlineStr">
+      <c r="A323" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B323" s="2" t="inlineStr">
         <is>
           <t>B2-D2</t>
         </is>
       </c>
-      <c r="C323" s="5" t="inlineStr">
+      <c r="C323" s="2" t="inlineStr">
         <is>
           <t>RHEUMATOLOGY</t>
         </is>
       </c>
-      <c r="D323" s="5" t="inlineStr">
+      <c r="D323" s="2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E323" s="5" t="inlineStr">
+      <c r="E323" s="2" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F323" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G323" s="5" t="inlineStr"/>
-      <c r="H323" s="5" t="inlineStr">
-        <is>
-          <t>0/61</t>
-        </is>
-      </c>
-      <c r="I323" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F323" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G323" s="2" t="inlineStr"/>
+      <c r="H323" s="2" t="inlineStr">
+        <is>
+          <t>35/61</t>
+        </is>
+      </c>
+      <c r="I323" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 16:07:05 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
@@ -950,7 +950,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>85.4%</t>
+          <t>86.0%</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>71.4%</t>
+          <t>71.5%</t>
         </is>
       </c>
     </row>
@@ -1600,17 +1600,17 @@
         <v>40</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P19" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q19" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R19" s="4" t="inlineStr">
         <is>
-          <t>85.0%</t>
+          <t>87.5%</t>
         </is>
       </c>
       <c r="S19" s="4" t="inlineStr">
@@ -1678,22 +1678,22 @@
         <v>42</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P20" s="4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R20" s="4" t="inlineStr">
         <is>
-          <t>78.6%</t>
+          <t>81.0%</t>
         </is>
       </c>
       <c r="S20" s="4" t="inlineStr">
         <is>
-          <t>73.4%</t>
+          <t>74.0%</t>
         </is>
       </c>
     </row>
@@ -8754,45 +8754,49 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B180" s="5" t="inlineStr">
+      <c r="A180" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B180" s="2" t="inlineStr">
         <is>
           <t>B2-C1</t>
         </is>
       </c>
-      <c r="C180" s="5" t="inlineStr">
+      <c r="C180" s="2" t="inlineStr">
         <is>
           <t>GASTROENTEROLOGY</t>
         </is>
       </c>
-      <c r="D180" s="5" t="inlineStr">
+      <c r="D180" s="2" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E180" s="5" t="inlineStr">
+      <c r="E180" s="2" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F180" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G180" s="5" t="inlineStr"/>
-      <c r="H180" s="5" t="inlineStr">
-        <is>
-          <t>0/52</t>
-        </is>
-      </c>
-      <c r="I180" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F180" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G180" s="2" t="inlineStr">
+        <is>
+          <t>emp17066@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H180" s="2" t="inlineStr">
+        <is>
+          <t>37/52</t>
+        </is>
+      </c>
+      <c r="I180" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -10173,45 +10177,49 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B213" s="5" t="inlineStr">
+      <c r="A213" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B213" s="2" t="inlineStr">
         <is>
           <t>B2-C2</t>
         </is>
       </c>
-      <c r="C213" s="5" t="inlineStr">
+      <c r="C213" s="2" t="inlineStr">
         <is>
           <t>GASTROENTEROLOGY</t>
         </is>
       </c>
-      <c r="D213" s="5" t="inlineStr">
+      <c r="D213" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E213" s="5" t="inlineStr">
+      <c r="E213" s="2" t="inlineStr">
         <is>
           <t>18/01/2026</t>
         </is>
       </c>
-      <c r="F213" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G213" s="5" t="inlineStr"/>
-      <c r="H213" s="5" t="inlineStr">
-        <is>
-          <t>0/51</t>
-        </is>
-      </c>
-      <c r="I213" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F213" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G213" s="2" t="inlineStr">
+        <is>
+          <t>emp17066@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H213" s="2" t="inlineStr">
+        <is>
+          <t>48/51</t>
+        </is>
+      </c>
+      <c r="I213" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 17:16:42 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -576,7 +576,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr"/>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
           <t>18/25</t>
@@ -624,7 +628,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
           <t>20/25</t>
@@ -677,7 +685,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr"/>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
           <t>20/25</t>
@@ -728,7 +740,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr"/>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
           <t>18/25</t>
@@ -779,7 +795,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr"/>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
           <t>22/25</t>
@@ -796,7 +816,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7">
@@ -830,7 +850,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G7" s="2" t="inlineStr"/>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
           <t>22/25</t>
@@ -847,7 +871,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
@@ -881,7 +905,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G8" s="2" t="inlineStr"/>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
           <t>23/25</t>
@@ -932,7 +960,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr"/>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
           <t>21/25</t>
@@ -950,7 +982,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>86.0%</t>
+          <t>86.6%</t>
         </is>
       </c>
     </row>
@@ -985,7 +1017,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G10" s="2" t="inlineStr"/>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
           <t>22/25</t>
@@ -1003,7 +1039,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>71.5%</t>
+          <t>71.4%</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1074,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G11" s="2" t="inlineStr"/>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
           <t>18/25</t>
@@ -1444,22 +1484,22 @@
         <v>40</v>
       </c>
       <c r="O17" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P17" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q17" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R17" s="4" t="inlineStr">
         <is>
-          <t>92.5%</t>
+          <t>95.0%</t>
         </is>
       </c>
       <c r="S17" s="4" t="inlineStr">
         <is>
-          <t>71.4%</t>
+          <t>70.5%</t>
         </is>
       </c>
     </row>
@@ -1522,22 +1562,22 @@
         <v>40</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P18" s="4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q18" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R18" s="4" t="inlineStr">
         <is>
-          <t>82.5%</t>
+          <t>85.0%</t>
         </is>
       </c>
       <c r="S18" s="4" t="inlineStr">
         <is>
-          <t>70.3%</t>
+          <t>70.4%</t>
         </is>
       </c>
     </row>
@@ -2786,7 +2826,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G42" s="2" t="inlineStr"/>
+      <c r="G42" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H42" s="2" t="inlineStr">
         <is>
           <t>17/23</t>
@@ -2829,7 +2873,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G43" s="2" t="inlineStr"/>
+      <c r="G43" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
           <t>22/23</t>
@@ -2872,7 +2920,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G44" s="2" t="inlineStr"/>
+      <c r="G44" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
           <t>22/23</t>
@@ -2915,7 +2967,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G45" s="2" t="inlineStr"/>
+      <c r="G45" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
           <t>19/23</t>
@@ -2958,7 +3014,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G46" s="2" t="inlineStr"/>
+      <c r="G46" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
           <t>21/23</t>
@@ -3001,7 +3061,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G47" s="2" t="inlineStr"/>
+      <c r="G47" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
           <t>19/23</t>
@@ -3044,7 +3108,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G48" s="2" t="inlineStr"/>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
           <t>21/23</t>
@@ -3087,7 +3155,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G49" s="2" t="inlineStr"/>
+      <c r="G49" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H49" s="2" t="inlineStr">
         <is>
           <t>23/23</t>
@@ -3130,7 +3202,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G50" s="2" t="inlineStr"/>
+      <c r="G50" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H50" s="2" t="inlineStr">
         <is>
           <t>21/23</t>
@@ -3173,7 +3249,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G51" s="2" t="inlineStr"/>
+      <c r="G51" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H51" s="2" t="inlineStr">
         <is>
           <t>19/23</t>
@@ -4741,7 +4821,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G87" s="2" t="inlineStr"/>
+      <c r="G87" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H87" s="2" t="inlineStr">
         <is>
           <t>15/40</t>
@@ -4883,45 +4967,45 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B91" s="5" t="inlineStr">
+      <c r="A91" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B91" s="2" t="inlineStr">
         <is>
           <t>B2-B1</t>
         </is>
       </c>
-      <c r="C91" s="5" t="inlineStr">
+      <c r="C91" s="2" t="inlineStr">
         <is>
           <t>ENDOCRINOLOGY</t>
         </is>
       </c>
-      <c r="D91" s="5" t="inlineStr">
+      <c r="D91" s="2" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E91" s="5" t="inlineStr">
+      <c r="E91" s="2" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F91" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G91" s="5" t="inlineStr"/>
-      <c r="H91" s="5" t="inlineStr">
-        <is>
-          <t>0/40</t>
-        </is>
-      </c>
-      <c r="I91" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F91" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G91" s="2" t="inlineStr"/>
+      <c r="H91" s="2" t="inlineStr">
+        <is>
+          <t>16/40</t>
+        </is>
+      </c>
+      <c r="I91" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -6481,7 +6565,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G127" s="2" t="inlineStr"/>
+      <c r="G127" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H127" s="2" t="inlineStr">
         <is>
           <t>20/35</t>
@@ -6623,45 +6711,45 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B131" s="5" t="inlineStr">
+      <c r="A131" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B131" s="2" t="inlineStr">
         <is>
           <t>B2-B2</t>
         </is>
       </c>
-      <c r="C131" s="5" t="inlineStr">
+      <c r="C131" s="2" t="inlineStr">
         <is>
           <t>ENDOCRINOLOGY</t>
         </is>
       </c>
-      <c r="D131" s="5" t="inlineStr">
+      <c r="D131" s="2" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E131" s="5" t="inlineStr">
+      <c r="E131" s="2" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F131" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G131" s="5" t="inlineStr"/>
-      <c r="H131" s="5" t="inlineStr">
-        <is>
-          <t>0/35</t>
-        </is>
-      </c>
-      <c r="I131" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F131" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G131" s="2" t="inlineStr"/>
+      <c r="H131" s="2" t="inlineStr">
+        <is>
+          <t>26/35</t>
+        </is>
+      </c>
+      <c r="I131" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -8006,7 +8094,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G162" s="2" t="inlineStr"/>
+      <c r="G162" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H162" s="2" t="inlineStr">
         <is>
           <t>45/52</t>
@@ -8049,7 +8141,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G163" s="2" t="inlineStr"/>
+      <c r="G163" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H163" s="2" t="inlineStr">
         <is>
           <t>43/52</t>
@@ -8092,7 +8188,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G164" s="2" t="inlineStr"/>
+      <c r="G164" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H164" s="2" t="inlineStr">
         <is>
           <t>51/52</t>
@@ -8135,7 +8235,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G165" s="2" t="inlineStr"/>
+      <c r="G165" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H165" s="2" t="inlineStr">
         <is>
           <t>46/52</t>
@@ -8221,7 +8325,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G167" s="2" t="inlineStr"/>
+      <c r="G167" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H167" s="2" t="inlineStr">
         <is>
           <t>33/52</t>
@@ -8264,7 +8372,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G168" s="2" t="inlineStr"/>
+      <c r="G168" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H168" s="2" t="inlineStr">
         <is>
           <t>48/52</t>
@@ -8307,7 +8419,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G169" s="2" t="inlineStr"/>
+      <c r="G169" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H169" s="2" t="inlineStr">
         <is>
           <t>46/52</t>
@@ -8350,7 +8466,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G170" s="2" t="inlineStr"/>
+      <c r="G170" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H170" s="2" t="inlineStr">
         <is>
           <t>51/52</t>
@@ -8393,7 +8513,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G171" s="2" t="inlineStr"/>
+      <c r="G171" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H171" s="2" t="inlineStr">
         <is>
           <t>47/52</t>
@@ -9734,7 +9858,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G202" s="2" t="inlineStr"/>
+      <c r="G202" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H202" s="2" t="inlineStr">
         <is>
           <t>44/51</t>
@@ -9777,7 +9905,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G203" s="2" t="inlineStr"/>
+      <c r="G203" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H203" s="2" t="inlineStr">
         <is>
           <t>41/51</t>
@@ -9820,7 +9952,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G204" s="2" t="inlineStr"/>
+      <c r="G204" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H204" s="2" t="inlineStr">
         <is>
           <t>49/51</t>
@@ -9863,7 +9999,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G205" s="2" t="inlineStr"/>
+      <c r="G205" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H205" s="2" t="inlineStr">
         <is>
           <t>47/51</t>
@@ -9949,7 +10089,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G207" s="2" t="inlineStr"/>
+      <c r="G207" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H207" s="2" t="inlineStr">
         <is>
           <t>34/51</t>
@@ -9992,7 +10136,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G208" s="2" t="inlineStr"/>
+      <c r="G208" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H208" s="2" t="inlineStr">
         <is>
           <t>48/51</t>
@@ -10035,7 +10183,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G209" s="2" t="inlineStr"/>
+      <c r="G209" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H209" s="2" t="inlineStr">
         <is>
           <t>46/51</t>
@@ -10078,7 +10230,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G210" s="2" t="inlineStr"/>
+      <c r="G210" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H210" s="2" t="inlineStr">
         <is>
           <t>43/51</t>
@@ -10121,7 +10277,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G211" s="2" t="inlineStr"/>
+      <c r="G211" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H211" s="2" t="inlineStr">
         <is>
           <t>47/51</t>
@@ -11552,7 +11712,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G244" s="2" t="inlineStr"/>
+      <c r="G244" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H244" s="2" t="inlineStr">
         <is>
           <t>26/28</t>
@@ -11595,7 +11759,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G245" s="2" t="inlineStr"/>
+      <c r="G245" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H245" s="2" t="inlineStr">
         <is>
           <t>20/28</t>
@@ -11638,7 +11806,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G246" s="2" t="inlineStr"/>
+      <c r="G246" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H246" s="2" t="inlineStr">
         <is>
           <t>26/28</t>
@@ -11681,7 +11853,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G247" s="2" t="inlineStr"/>
+      <c r="G247" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H247" s="2" t="inlineStr">
         <is>
           <t>25/28</t>
@@ -11724,7 +11900,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G248" s="2" t="inlineStr"/>
+      <c r="G248" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H248" s="2" t="inlineStr">
         <is>
           <t>27/28</t>
@@ -11767,7 +11947,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G249" s="2" t="inlineStr"/>
+      <c r="G249" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H249" s="2" t="inlineStr">
         <is>
           <t>22/28</t>
@@ -11810,7 +11994,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G250" s="2" t="inlineStr"/>
+      <c r="G250" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H250" s="2" t="inlineStr">
         <is>
           <t>26/28</t>
@@ -11853,7 +12041,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G251" s="2" t="inlineStr"/>
+      <c r="G251" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H251" s="2" t="inlineStr">
         <is>
           <t>25/28</t>
@@ -11896,7 +12088,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G252" s="2" t="inlineStr"/>
+      <c r="G252" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H252" s="2" t="inlineStr">
         <is>
           <t>26/28</t>
@@ -11939,7 +12135,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G253" s="2" t="inlineStr"/>
+      <c r="G253" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H253" s="2" t="inlineStr">
         <is>
           <t>24/28</t>
@@ -13284,7 +13484,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G284" s="2" t="inlineStr"/>
+      <c r="G284" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H284" s="2" t="inlineStr">
         <is>
           <t>40/61</t>
@@ -13327,7 +13531,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G285" s="2" t="inlineStr"/>
+      <c r="G285" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H285" s="2" t="inlineStr">
         <is>
           <t>41/61</t>
@@ -13370,7 +13578,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G286" s="2" t="inlineStr"/>
+      <c r="G286" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H286" s="2" t="inlineStr">
         <is>
           <t>42/61</t>
@@ -13413,7 +13625,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G287" s="2" t="inlineStr"/>
+      <c r="G287" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H287" s="2" t="inlineStr">
         <is>
           <t>39/61</t>
@@ -13456,7 +13672,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G288" s="2" t="inlineStr"/>
+      <c r="G288" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H288" s="2" t="inlineStr">
         <is>
           <t>40/61</t>
@@ -13499,7 +13719,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G289" s="2" t="inlineStr"/>
+      <c r="G289" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H289" s="2" t="inlineStr">
         <is>
           <t>33/61</t>
@@ -13542,7 +13766,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G290" s="2" t="inlineStr"/>
+      <c r="G290" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H290" s="2" t="inlineStr">
         <is>
           <t>36/61</t>
@@ -13585,7 +13813,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G291" s="2" t="inlineStr"/>
+      <c r="G291" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H291" s="2" t="inlineStr">
         <is>
           <t>45/61</t>
@@ -13628,7 +13860,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G292" s="2" t="inlineStr"/>
+      <c r="G292" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H292" s="2" t="inlineStr">
         <is>
           <t>42/61</t>
@@ -13671,7 +13907,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G293" s="2" t="inlineStr"/>
+      <c r="G293" s="2" t="inlineStr">
+        <is>
+          <t>776626600547</t>
+        </is>
+      </c>
       <c r="H293" s="2" t="inlineStr">
         <is>
           <t>43/61</t>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 18:25:14 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -816,7 +816,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
@@ -982,7 +982,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>86.6%</t>
+          <t>87.0%</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>71.4%</t>
+          <t>71.3%</t>
         </is>
       </c>
     </row>
@@ -1796,22 +1796,22 @@
         <v>40</v>
       </c>
       <c r="O21" s="4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P21" s="4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R21" s="4" t="inlineStr">
         <is>
-          <t>77.5%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="S21" s="4" t="inlineStr">
         <is>
-          <t>69.4%</t>
+          <t>68.6%</t>
         </is>
       </c>
     </row>
@@ -12486,7 +12486,7 @@
       <c r="G261" s="2" t="inlineStr"/>
       <c r="H261" s="2" t="inlineStr">
         <is>
-          <t>1/28</t>
+          <t>4/28</t>
         </is>
       </c>
       <c r="I261" s="2" t="inlineStr">
@@ -12496,45 +12496,45 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B262" s="5" t="inlineStr">
+      <c r="A262" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B262" s="2" t="inlineStr">
         <is>
           <t>B2-D1</t>
         </is>
       </c>
-      <c r="C262" s="5" t="inlineStr">
+      <c r="C262" s="2" t="inlineStr">
         <is>
           <t>GASTROENTEROLOGY</t>
         </is>
       </c>
-      <c r="D262" s="5" t="inlineStr">
+      <c r="D262" s="2" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E262" s="5" t="inlineStr">
+      <c r="E262" s="2" t="inlineStr">
         <is>
           <t>13/01/2026</t>
         </is>
       </c>
-      <c r="F262" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G262" s="5" t="inlineStr"/>
-      <c r="H262" s="5" t="inlineStr">
-        <is>
-          <t>0/28</t>
-        </is>
-      </c>
-      <c r="I262" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F262" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G262" s="2" t="inlineStr"/>
+      <c r="H262" s="2" t="inlineStr">
+        <is>
+          <t>10/28</t>
+        </is>
+      </c>
+      <c r="I262" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -14301,7 +14301,7 @@
       <c r="G302" s="2" t="inlineStr"/>
       <c r="H302" s="2" t="inlineStr">
         <is>
-          <t>40/61</t>
+          <t>41/61</t>
         </is>
       </c>
       <c r="I302" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 10:52:26 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
+++ b/attendance_reports/Y5_B2526_General_&_Special_Internal_2_B2_session_analysis.xlsx
@@ -816,7 +816,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
@@ -982,7 +982,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>87.6%</t>
+          <t>87.9%</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>71.1%</t>
+          <t>71.2%</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="S15" s="4" t="inlineStr">
         <is>
-          <t>79.1%</t>
+          <t>79.7%</t>
         </is>
       </c>
     </row>
@@ -1406,22 +1406,22 @@
         <v>40</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P16" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q16" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R16" s="4" t="inlineStr">
         <is>
-          <t>85.0%</t>
+          <t>87.5%</t>
         </is>
       </c>
       <c r="S16" s="4" t="inlineStr">
         <is>
-          <t>82.1%</t>
+          <t>82.4%</t>
         </is>
       </c>
     </row>
@@ -2548,7 +2548,7 @@
       <c r="G35" s="2" t="inlineStr"/>
       <c r="H35" s="2" t="inlineStr">
         <is>
-          <t>14/25</t>
+          <t>19/25</t>
         </is>
       </c>
       <c r="I35" s="2" t="inlineStr">
@@ -4311,45 +4311,45 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="5" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-      <c r="B75" s="5" t="inlineStr">
+      <c r="A75" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B75" s="2" t="inlineStr">
         <is>
           <t>B2-A2</t>
         </is>
       </c>
-      <c r="C75" s="5" t="inlineStr">
+      <c r="C75" s="2" t="inlineStr">
         <is>
           <t>PHYSICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D75" s="5" t="inlineStr">
+      <c r="D75" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E75" s="5" t="inlineStr">
+      <c r="E75" s="2" t="inlineStr">
         <is>
           <t>21/01/2026</t>
         </is>
       </c>
-      <c r="F75" s="5" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G75" s="5" t="inlineStr"/>
-      <c r="H75" s="5" t="inlineStr">
-        <is>
-          <t>0/23</t>
-        </is>
-      </c>
-      <c r="I75" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F75" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G75" s="2" t="inlineStr"/>
+      <c r="H75" s="2" t="inlineStr">
+        <is>
+          <t>21/23</t>
+        </is>
+      </c>
+      <c r="I75" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>